<commit_message>
Improve the example aproda report
</commit_message>
<xml_diff>
--- a/budgeteer-aproda-importer/src/main/resources/example_aproda_report.xlsx
+++ b/budgeteer-aproda-importer/src/main/resources/example_aproda_report.xlsx
@@ -1,50 +1,49 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trzpiot\Documents\Workspace\budgeteer\budgeteer-aproda-importer\src\main\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <workbookProtection lockWindows="1"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="372" firstSheet="0" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="372" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Arbeitspakete" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Arbeitspakete PM" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Aufwände gesamt" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Arbeitspakete" sheetId="1" r:id="rId1"/>
+    <sheet name="Arbeitspakete PM" sheetId="2" r:id="rId2"/>
+    <sheet name="Aufwände gesamt" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles" vbProcedure="false">Arbeitspakete!$1:$4</definedName>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Arbeitspakete!$A$3:$M$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles" vbProcedure="false">'Arbeitspakete PM'!$1:$4</definedName>
-    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'Arbeitspakete PM'!$A$3:$G$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Titles" vbProcedure="false">'Aufwände gesamt'!$1:$4</definedName>
-    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">'Aufwände gesamt'!$A$3:$J$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles" vbProcedure="false">Arbeitspakete!$1:$4</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0" vbProcedure="false">Arbeitspakete!$1:$4</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0" vbProcedure="false">Arbeitspakete!$1:$4</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0" vbProcedure="false">Arbeitspakete!$1:$4</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Arbeitspakete!$A$3:$M$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Arbeitspakete!$A$3:$M$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Arbeitspakete!$A$3:$M$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Arbeitspakete!$A$3:$M$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles" vbProcedure="false">'Arbeitspakete PM'!$1:$4</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0" vbProcedure="false">'Arbeitspakete PM'!$1:$4</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0_0" vbProcedure="false">'Arbeitspakete PM'!$1:$4</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0_0_0" vbProcedure="false">'Arbeitspakete PM'!$1:$4</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'Arbeitspakete PM'!$A$3:$G$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Arbeitspakete PM'!$A$3:$G$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Arbeitspakete PM'!$A$3:$G$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Arbeitspakete PM'!$A$3:$G$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Titles" vbProcedure="false">'Aufwände gesamt'!$1:$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Titles_0" vbProcedure="false">'Aufwände gesamt'!$1:$4</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Titles_0_0" vbProcedure="false">'Aufwände gesamt'!$1:$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Titles_0_0_0" vbProcedure="false">'Aufwände gesamt'!$1:$4</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">'Aufwände gesamt'!$A$3:$J$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Aufwände gesamt'!$A$3:$J$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Aufwände gesamt'!$A$3:$J$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Aufwände gesamt'!$A$3:$J$3</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="0">Arbeitspakete!$A$3:$M$3</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="1">'Arbeitspakete PM'!$A$3:$G$3</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="2">'Aufwände gesamt'!$A$3:$J$3</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="0">Arbeitspakete!$A$3:$M$3</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="1">'Arbeitspakete PM'!$A$3:$G$3</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="2">'Aufwände gesamt'!$A$3:$J$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="0">Arbeitspakete!$A$3:$M$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="1">'Arbeitspakete PM'!$A$3:$G$3</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="2">'Aufwände gesamt'!$A$3:$J$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0">Arbeitspakete!$A$3:$M$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1">'Arbeitspakete PM'!$A$3:$G$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2">'Aufwände gesamt'!$A$3:$J$3</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Arbeitspakete!$1:$4</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="1">'Arbeitspakete PM'!$1:$4</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="2">'Aufwände gesamt'!$1:$3</definedName>
+    <definedName name="Print_Titles_0" localSheetId="0">Arbeitspakete!$1:$4</definedName>
+    <definedName name="Print_Titles_0" localSheetId="1">'Arbeitspakete PM'!$1:$4</definedName>
+    <definedName name="Print_Titles_0" localSheetId="2">'Aufwände gesamt'!$1:$4</definedName>
+    <definedName name="Print_Titles_0_0" localSheetId="0">Arbeitspakete!$1:$4</definedName>
+    <definedName name="Print_Titles_0_0" localSheetId="1">'Arbeitspakete PM'!$1:$4</definedName>
+    <definedName name="Print_Titles_0_0" localSheetId="2">'Aufwände gesamt'!$1:$3</definedName>
+    <definedName name="Print_Titles_0_0_0" localSheetId="0">Arbeitspakete!$1:$4</definedName>
+    <definedName name="Print_Titles_0_0_0" localSheetId="1">'Arbeitspakete PM'!$1:$4</definedName>
+    <definedName name="Print_Titles_0_0_0" localSheetId="2">'Aufwände gesamt'!$1:$4</definedName>
   </definedNames>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -102,13 +101,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
-    <numFmt numFmtId="166" formatCode="#,##0.0&quot; h&quot;"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0.0&quot; h&quot;"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -116,22 +113,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -144,7 +126,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
@@ -167,88 +149,51 @@
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -307,17 +252,29 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>5</xdr:col>
@@ -333,11 +290,11 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="Picture 1" descr=""/>
+        <xdr:cNvPr id="2" name="Picture 1"/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -360,141 +317,382 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
-    <pageSetUpPr fitToPage="true"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.77551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.780612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.780612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.780612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="12.780612244898"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.7755102040816"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.780612244898"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.7857142857143"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="12.780612244898"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="13.780612244898"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.780612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.72959183673469"/>
+    <col min="1" max="1" width="5.77734375"/>
+    <col min="2" max="2" width="20.77734375"/>
+    <col min="3" max="3" width="13.77734375"/>
+    <col min="4" max="4" width="36.77734375"/>
+    <col min="5" max="6" width="12.77734375"/>
+    <col min="7" max="7" width="22.77734375"/>
+    <col min="8" max="8" width="12.77734375"/>
+    <col min="9" max="9" width="15.77734375"/>
+    <col min="10" max="11" width="12.77734375"/>
+    <col min="12" max="12" width="13.77734375"/>
+    <col min="13" max="13" width="11.77734375"/>
+    <col min="14" max="1025" width="8.77734375"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A3:M3"/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="0" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" fitToHeight="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
-    <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
+    <sheetView windowProtection="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.77551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.780612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.7755102040816"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="40.7755102040816"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.780612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.7857142857143"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.780612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.72959183673469"/>
+    <col min="1" max="1" width="6.77734375"/>
+    <col min="2" max="2" width="17.77734375"/>
+    <col min="3" max="3" width="14.77734375"/>
+    <col min="4" max="4" width="40.77734375"/>
+    <col min="5" max="5" width="13.77734375"/>
+    <col min="6" max="6" width="16.77734375"/>
+    <col min="7" max="7" width="20.77734375"/>
+    <col min="8" max="1025" width="8.77734375"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A3:G3"/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
-    <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J65536"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="J11" activeCellId="0" sqref="J11"/>
+    <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.780612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.780612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.7755102040816"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.780612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="15.7857142857143"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="49.7857142857143"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.780612244898"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.77551020408163"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="21.780612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.72959183673469"/>
+    <col min="1" max="1" width="26.77734375"/>
+    <col min="2" max="2" width="10.77734375"/>
+    <col min="3" max="3" width="14.77734375"/>
+    <col min="4" max="4" width="30.77734375"/>
+    <col min="5" max="6" width="15.77734375"/>
+    <col min="7" max="7" width="49.77734375"/>
+    <col min="8" max="8" width="13.77734375"/>
+    <col min="9" max="9" width="6.77734375"/>
+    <col min="10" max="10" width="21.77734375"/>
+    <col min="11" max="1025" width="8.77734375"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -526,12 +724,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="6" t="n">
-        <v>41918</v>
+      <c r="B4" s="6">
+        <f t="shared" ref="B4:B9" ca="1" si="0">B5-IF(WEEKDAY(B5,2)=1,3,1)</f>
+        <v>43313</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>12</v>
@@ -548,7 +747,7 @@
       <c r="G4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="7" t="n">
+      <c r="H4" s="7">
         <v>9</v>
       </c>
       <c r="I4" s="5" t="s">
@@ -558,12 +757,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="6" t="n">
-        <v>41920</v>
+      <c r="B5" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>43314</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>12</v>
@@ -580,7 +780,7 @@
       <c r="G5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="7" t="n">
+      <c r="H5" s="7">
         <v>7</v>
       </c>
       <c r="I5" s="5" t="s">
@@ -590,12 +790,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="6" t="n">
-        <v>41925</v>
+      <c r="B6" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>43315</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>12</v>
@@ -612,7 +813,7 @@
       <c r="G6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="7" t="n">
+      <c r="H6" s="7">
         <v>7</v>
       </c>
       <c r="I6" s="5" t="s">
@@ -622,12 +823,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="6" t="n">
-        <v>41939</v>
+      <c r="B7" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>43318</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>12</v>
@@ -644,7 +846,7 @@
       <c r="G7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="7" t="n">
+      <c r="H7" s="7">
         <v>8</v>
       </c>
       <c r="I7" s="5" t="s">
@@ -654,12 +856,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="6" t="n">
-        <v>41940</v>
+      <c r="B8" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>43319</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>12</v>
@@ -676,7 +879,7 @@
       <c r="G8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H8" s="7" t="n">
+      <c r="H8" s="7">
         <v>8</v>
       </c>
       <c r="I8" s="5" t="s">
@@ -686,12 +889,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="6" t="n">
-        <v>41941</v>
+      <c r="B9" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>43320</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>12</v>
@@ -708,7 +912,7 @@
       <c r="G9" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="7" t="n">
+      <c r="H9" s="7">
         <v>8.5</v>
       </c>
       <c r="I9" s="5" t="s">
@@ -718,12 +922,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="6" t="n">
-        <v>41942</v>
+      <c r="B10" s="6">
+        <f ca="1">B11-IF(WEEKDAY(B11,2)=1,3,1)</f>
+        <v>43321</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>12</v>
@@ -740,7 +945,7 @@
       <c r="G10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="7" t="n">
+      <c r="H10" s="7">
         <v>8.5</v>
       </c>
       <c r="I10" s="5" t="s">
@@ -750,12 +955,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="6" t="n">
-        <v>41943</v>
+      <c r="B11" s="6">
+        <f ca="1">TODAY()</f>
+        <v>43322</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>12</v>
@@ -772,7 +978,7 @@
       <c r="G11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H11" s="7" t="n">
+      <c r="H11" s="7">
         <v>8</v>
       </c>
       <c r="I11" s="5" t="s">
@@ -782,32 +988,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1006" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <autoFilter ref="A3:J3"/>
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>
   </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add calculation of dates for the example file example_aproda_report
</commit_message>
<xml_diff>
--- a/budgeteer-aproda-importer/src/main/resources/example_aproda_report.xlsx
+++ b/budgeteer-aproda-importer/src/main/resources/example_aproda_report.xlsx
@@ -89,13 +89,13 @@
     <t>not relevant</t>
   </si>
   <si>
-    <t>Budget 1</t>
-  </si>
-  <si>
     <t>Ja</t>
   </si>
   <si>
-    <t>Budget 2</t>
+    <t>Testmanagement</t>
+  </si>
+  <si>
+    <t>Scratch the Cat</t>
   </si>
 </sst>
 </file>
@@ -177,9 +177,6 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -188,6 +185,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -608,7 +608,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -644,7 +644,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -665,7 +665,7 @@
   <sheetViews>
     <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
+      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -683,308 +683,284 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+      <c r="A1" s="7"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
     </row>
     <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
+      <c r="A2" s="2"/>
     </row>
     <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="6">
-        <f t="shared" ref="B4:B9" ca="1" si="0">B5-IF(WEEKDAY(B5,2)=1,3,1)</f>
-        <v>43313</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="5" t="s">
+      <c r="B4" s="5"/>
+      <c r="C4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="6">
+        <v>9</v>
+      </c>
+      <c r="I4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="7">
-        <v>9</v>
-      </c>
-      <c r="I4" s="5" t="s">
+      <c r="J4" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="G5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="6">
+        <v>7</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>43314</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="5" t="s">
+      <c r="B6" s="5"/>
+      <c r="C6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="6">
+        <v>7</v>
+      </c>
+      <c r="I6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="7">
-        <v>7</v>
-      </c>
-      <c r="I5" s="5" t="s">
+      <c r="J6" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="J5" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="G7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="6">
+        <v>8</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>43315</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="5" t="s">
+      <c r="B8" s="5"/>
+      <c r="C8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="6">
+        <v>8</v>
+      </c>
+      <c r="I8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="7">
-        <v>7</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="J8" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>43318</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="5" t="s">
+      <c r="B9" s="5"/>
+      <c r="C9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="6">
+        <v>8.5</v>
+      </c>
+      <c r="I9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" s="7">
+      <c r="J9" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="6">
+        <v>8.5</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" s="6">
         <v>8</v>
       </c>
-      <c r="I7" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>43319</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" s="7">
-        <v>8</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>43320</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H9" s="7">
-        <v>8.5</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="J9" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="6">
-        <f ca="1">B11-IF(WEEKDAY(B11,2)=1,3,1)</f>
-        <v>43321</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H10" s="7">
-        <v>8.5</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="6">
-        <f ca="1">TODAY()</f>
-        <v>43322</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H11" s="7">
-        <v>8</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="J11" s="5" t="s">
+      <c r="I11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J11" s="4" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>